<commit_message>
Distinguish between 'T_settle_filter' and 'T_settle_deque'
</commit_message>
<xml_diff>
--- a/FIR_filter_convolution_scheme.xlsx
+++ b/FIR_filter_convolution_scheme.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\_GitHub_repo\DvG_Arduino_lock-in_amp\filter_design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\_GitHub_repo\DvG_Arduino_lock-in_amp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEABC4BA-DBB4-49C7-8811-D10C313F0B4D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA5241C-C5FD-477D-880A-100D47EEF298}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9828" yWindow="3252" windowWidth="16536" windowHeight="10128" xr2:uid="{954ABCBC-5CDF-4E6C-ABB2-AE0B044014B7}"/>
+    <workbookView xWindow="4848" yWindow="3048" windowWidth="20664" windowHeight="12660" xr2:uid="{954ABCBC-5CDF-4E6C-ABB2-AE0B044014B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$BE$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$BE$55</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="66">
   <si>
     <t>N_taps</t>
   </si>
@@ -225,7 +225,19 @@
     <t>= win_idx_valid_start / Fs</t>
   </si>
   <si>
-    <t>T_delay_valid_start</t>
+    <t>i.e. Filter settling time</t>
+  </si>
+  <si>
+    <t>i.e. Deque settling time</t>
+  </si>
+  <si>
+    <t>T_settle_filter</t>
+  </si>
+  <si>
+    <t>T_settle_deque</t>
+  </si>
+  <si>
+    <t>= T_settle_filter * 2</t>
   </si>
 </sst>
 </file>
@@ -316,7 +328,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -477,11 +489,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -616,6 +646,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -625,7 +662,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -943,10 +979,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BE77"/>
+  <dimension ref="A1:BE78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -979,54 +1015,54 @@
       <c r="F4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="61"/>
-      <c r="P4" s="62"/>
-      <c r="Q4" s="60" t="s">
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="67"/>
+      <c r="Q4" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="61"/>
-      <c r="S4" s="61"/>
-      <c r="T4" s="61"/>
-      <c r="U4" s="61"/>
-      <c r="V4" s="61"/>
-      <c r="W4" s="61"/>
-      <c r="X4" s="61"/>
-      <c r="Y4" s="61"/>
-      <c r="Z4" s="62"/>
-      <c r="AA4" s="60" t="s">
+      <c r="R4" s="66"/>
+      <c r="S4" s="66"/>
+      <c r="T4" s="66"/>
+      <c r="U4" s="66"/>
+      <c r="V4" s="66"/>
+      <c r="W4" s="66"/>
+      <c r="X4" s="66"/>
+      <c r="Y4" s="66"/>
+      <c r="Z4" s="67"/>
+      <c r="AA4" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="AB4" s="61"/>
-      <c r="AC4" s="61"/>
-      <c r="AD4" s="61"/>
-      <c r="AE4" s="61"/>
-      <c r="AF4" s="61"/>
-      <c r="AG4" s="61"/>
-      <c r="AH4" s="61"/>
-      <c r="AI4" s="61"/>
-      <c r="AJ4" s="62"/>
-      <c r="AK4" s="60" t="s">
+      <c r="AB4" s="66"/>
+      <c r="AC4" s="66"/>
+      <c r="AD4" s="66"/>
+      <c r="AE4" s="66"/>
+      <c r="AF4" s="66"/>
+      <c r="AG4" s="66"/>
+      <c r="AH4" s="66"/>
+      <c r="AI4" s="66"/>
+      <c r="AJ4" s="67"/>
+      <c r="AK4" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="AL4" s="61"/>
-      <c r="AM4" s="61"/>
-      <c r="AN4" s="61"/>
-      <c r="AO4" s="61"/>
-      <c r="AP4" s="61"/>
-      <c r="AQ4" s="61"/>
-      <c r="AR4" s="61"/>
-      <c r="AS4" s="61"/>
-      <c r="AT4" s="62"/>
+      <c r="AL4" s="66"/>
+      <c r="AM4" s="66"/>
+      <c r="AN4" s="66"/>
+      <c r="AO4" s="66"/>
+      <c r="AP4" s="66"/>
+      <c r="AQ4" s="66"/>
+      <c r="AR4" s="66"/>
+      <c r="AS4" s="66"/>
+      <c r="AT4" s="67"/>
       <c r="AU4" s="4"/>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.3">
@@ -1746,66 +1782,66 @@
       <c r="F20" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="60" t="s">
+      <c r="G20" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="61"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="61"/>
-      <c r="L20" s="61"/>
-      <c r="M20" s="61"/>
-      <c r="N20" s="61"/>
-      <c r="O20" s="61"/>
-      <c r="P20" s="61"/>
-      <c r="Q20" s="60" t="s">
+      <c r="H20" s="66"/>
+      <c r="I20" s="66"/>
+      <c r="J20" s="66"/>
+      <c r="K20" s="66"/>
+      <c r="L20" s="66"/>
+      <c r="M20" s="66"/>
+      <c r="N20" s="66"/>
+      <c r="O20" s="66"/>
+      <c r="P20" s="66"/>
+      <c r="Q20" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="R20" s="61"/>
-      <c r="S20" s="61"/>
-      <c r="T20" s="61"/>
-      <c r="U20" s="61"/>
-      <c r="V20" s="61"/>
-      <c r="W20" s="61"/>
-      <c r="X20" s="61"/>
-      <c r="Y20" s="61"/>
-      <c r="Z20" s="61"/>
-      <c r="AA20" s="60" t="s">
+      <c r="R20" s="66"/>
+      <c r="S20" s="66"/>
+      <c r="T20" s="66"/>
+      <c r="U20" s="66"/>
+      <c r="V20" s="66"/>
+      <c r="W20" s="66"/>
+      <c r="X20" s="66"/>
+      <c r="Y20" s="66"/>
+      <c r="Z20" s="66"/>
+      <c r="AA20" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="AB20" s="61"/>
-      <c r="AC20" s="61"/>
-      <c r="AD20" s="61"/>
-      <c r="AE20" s="61"/>
-      <c r="AF20" s="61"/>
-      <c r="AG20" s="61"/>
-      <c r="AH20" s="61"/>
-      <c r="AI20" s="61"/>
-      <c r="AJ20" s="61"/>
-      <c r="AK20" s="60" t="s">
+      <c r="AB20" s="66"/>
+      <c r="AC20" s="66"/>
+      <c r="AD20" s="66"/>
+      <c r="AE20" s="66"/>
+      <c r="AF20" s="66"/>
+      <c r="AG20" s="66"/>
+      <c r="AH20" s="66"/>
+      <c r="AI20" s="66"/>
+      <c r="AJ20" s="66"/>
+      <c r="AK20" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="AL20" s="61"/>
-      <c r="AM20" s="61"/>
-      <c r="AN20" s="61"/>
-      <c r="AO20" s="61"/>
-      <c r="AP20" s="61"/>
-      <c r="AQ20" s="61"/>
-      <c r="AR20" s="61"/>
-      <c r="AS20" s="61"/>
-      <c r="AT20" s="61"/>
-      <c r="AU20" s="60" t="s">
+      <c r="AL20" s="66"/>
+      <c r="AM20" s="66"/>
+      <c r="AN20" s="66"/>
+      <c r="AO20" s="66"/>
+      <c r="AP20" s="66"/>
+      <c r="AQ20" s="66"/>
+      <c r="AR20" s="66"/>
+      <c r="AS20" s="66"/>
+      <c r="AT20" s="66"/>
+      <c r="AU20" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="AV20" s="61"/>
-      <c r="AW20" s="61"/>
-      <c r="AX20" s="61"/>
-      <c r="AY20" s="61"/>
-      <c r="AZ20" s="61"/>
-      <c r="BA20" s="61"/>
-      <c r="BB20" s="61"/>
-      <c r="BC20" s="61"/>
-      <c r="BD20" s="62"/>
+      <c r="AV20" s="66"/>
+      <c r="AW20" s="66"/>
+      <c r="AX20" s="66"/>
+      <c r="AY20" s="66"/>
+      <c r="AZ20" s="66"/>
+      <c r="BA20" s="66"/>
+      <c r="BB20" s="66"/>
+      <c r="BC20" s="66"/>
+      <c r="BD20" s="67"/>
       <c r="BE20" s="4"/>
     </row>
     <row r="21" spans="1:57" x14ac:dyDescent="0.3">
@@ -2946,14 +2982,14 @@
         <v>21</v>
       </c>
       <c r="B37" s="35">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="C37" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="63" t="s">
+      <c r="A38" s="60" t="s">
         <v>50</v>
       </c>
       <c r="B38" s="35">
@@ -2964,11 +3000,11 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="63" t="s">
+      <c r="A39" s="60" t="s">
         <v>22</v>
       </c>
       <c r="B39" s="35">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s">
         <v>26</v>
@@ -2980,7 +3016,7 @@
       </c>
       <c r="B41" s="43">
         <f>B38*B39</f>
-        <v>40500</v>
+        <v>20500</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
@@ -2995,7 +3031,7 @@
       </c>
       <c r="B42" s="43">
         <f>B38*(B39-1) + 1</f>
-        <v>40001</v>
+        <v>20001</v>
       </c>
       <c r="C42" t="s">
         <v>23</v>
@@ -3044,7 +3080,7 @@
       </c>
       <c r="B47" s="44">
         <f>B42*22*((B46-B45)/B37)</f>
-        <v>88.002200000000002</v>
+        <v>88.004400000000004</v>
       </c>
       <c r="C47" t="s">
         <v>29</v>
@@ -3053,13 +3089,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="53" t="s">
         <v>19</v>
       </c>
       <c r="B49" s="43">
         <f>B38+B42-1</f>
-        <v>40500</v>
+        <v>20500</v>
       </c>
       <c r="C49" s="54" t="s">
         <v>23</v>
@@ -3068,7 +3104,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="55" t="s">
         <v>18</v>
       </c>
@@ -3083,7 +3119,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="53" t="s">
         <v>27</v>
       </c>
@@ -3098,13 +3134,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="55" t="s">
         <v>2</v>
       </c>
       <c r="B52" s="43">
         <f>INT((B42-1)/2)</f>
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="C52" s="56" t="s">
         <v>23</v>
@@ -3113,13 +3149,13 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="53" t="s">
         <v>59</v>
       </c>
       <c r="B53" s="43">
         <f>B50+B52</f>
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="C53" s="54" t="s">
         <v>23</v>
@@ -3128,135 +3164,145 @@
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="55" t="s">
-        <v>61</v>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="62" t="s">
+        <v>63</v>
       </c>
       <c r="B54" s="44">
         <f>B53/B37</f>
         <v>2</v>
       </c>
-      <c r="C54" s="56" t="s">
+      <c r="C54" s="63" t="s">
         <v>28</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
+      <c r="F54" s="61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="64" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55" s="44">
+        <f>B54*2</f>
+        <v>4</v>
+      </c>
+      <c r="C55" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F55" s="61" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>21</v>
       </c>
-      <c r="B59" s="35">
+      <c r="B60" s="35">
         <v>10000</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>50</v>
       </c>
-      <c r="B60" s="35">
+      <c r="B61" s="35">
         <v>500</v>
       </c>
-      <c r="C60" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="C61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>0</v>
       </c>
-      <c r="B61" s="35">
+      <c r="B62" s="35">
         <v>9701</v>
       </c>
-      <c r="C61" t="s">
-        <v>23</v>
-      </c>
-      <c r="D61" s="1" t="s">
+      <c r="C62" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B62" s="23"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>22</v>
-      </c>
-      <c r="B63" s="43">
-        <f>1+(B61-1)/B60</f>
-        <v>20.399999999999999</v>
-      </c>
-      <c r="C63" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B63" s="23"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>22</v>
       </c>
       <c r="B64" s="43">
-        <f>_xlfn.CEILING.MATH(B63)</f>
-        <v>21</v>
+        <f>1+(B62-1)/B61</f>
+        <v>20.399999999999999</v>
       </c>
       <c r="C64" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" s="43">
+        <f>_xlfn.CEILING.MATH(B64)</f>
+        <v>21</v>
+      </c>
+      <c r="C65" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>54</v>
       </c>
-      <c r="B65" s="43">
-        <f>B60*B64</f>
+      <c r="B66" s="43">
+        <f>B61*B65</f>
         <v>10500</v>
       </c>
-      <c r="C65" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B66" s="51"/>
+      <c r="C66" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>44</v>
-      </c>
-      <c r="B67" s="33"/>
-      <c r="D67" t="s">
-        <v>43</v>
-      </c>
+      <c r="B67" s="51"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" s="35">
-        <v>49</v>
-      </c>
-      <c r="C68" t="s">
-        <v>24</v>
+        <v>44</v>
+      </c>
+      <c r="B68" s="33"/>
+      <c r="D68" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B69" s="35">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C69" t="s">
         <v>24</v>
@@ -3264,91 +3310,102 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>31</v>
+      </c>
+      <c r="B70" s="35">
+        <v>50</v>
+      </c>
+      <c r="C70" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>45</v>
       </c>
-      <c r="B70" s="44">
-        <f>B61*22*((B69-B68)/B59)</f>
+      <c r="B71" s="44">
+        <f>B62*22*((B70-B69)/B60)</f>
         <v>21.342200000000002</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>29</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="53" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B72" s="43">
-        <f>2*B75+B74</f>
+      <c r="B73" s="43">
+        <f>2*B76+B75</f>
         <v>10200</v>
       </c>
-      <c r="C72" s="54" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="55" t="s">
+      <c r="C73" s="54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="B73" s="43">
-        <f>B65-B72</f>
+      <c r="B74" s="43">
+        <f>B66-B73</f>
         <v>300</v>
       </c>
-      <c r="C73" s="56" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="53" t="s">
+      <c r="C74" s="56" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B74" s="43">
-        <f>B60</f>
+      <c r="B75" s="43">
+        <f>B61</f>
         <v>500</v>
       </c>
-      <c r="C74" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="D74" s="1" t="s">
+      <c r="C75" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="55" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B75" s="43">
-        <f>INT((B61-1)/2)</f>
+      <c r="B76" s="43">
+        <f>INT((B62-1)/2)</f>
         <v>4850</v>
       </c>
-      <c r="C75" s="56" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="53" t="s">
+      <c r="C76" s="56" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="B76" s="43">
-        <f>B75+B73</f>
+      <c r="B77" s="43">
+        <f>B76+B74</f>
         <v>5150</v>
       </c>
-      <c r="C76" s="54" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="B77" s="44">
-        <f>B76/B59</f>
+      <c r="C77" s="54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="B78" s="44">
+        <f>B77/B60</f>
         <v>0.51500000000000001</v>
       </c>
-      <c r="C77" s="56" t="s">
+      <c r="C78" s="56" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3367,7 +3424,7 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="54" max="56" man="1"/>
+    <brk id="55" max="56" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>